<commit_message>
Atualização automática diária da base
</commit_message>
<xml_diff>
--- a/base_despesas/2026/despesas_202601.xlsx
+++ b/base_despesas/2026/despesas_202601.xlsx
@@ -697,7 +697,7 @@
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -1995,7 +1995,7 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2231,7 +2231,7 @@
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3175,7 +3175,7 @@
       <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3293,7 +3293,7 @@
       <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3529,7 +3529,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3647,7 +3647,7 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4119,7 +4119,7 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4355,7 +4355,7 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4473,7 +4473,7 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4591,7 +4591,7 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4709,7 +4709,7 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4827,7 +4827,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -4945,7 +4945,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5063,7 +5063,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5181,7 +5181,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5299,7 +5299,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5535,7 +5535,7 @@
       <c r="AE43" t="inlineStr"/>
       <c r="AF43" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5653,7 +5653,7 @@
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5771,7 +5771,7 @@
       <c r="AE45" t="inlineStr"/>
       <c r="AF45" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6007,7 +6007,7 @@
       <c r="AE47" t="inlineStr"/>
       <c r="AF47" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6125,7 +6125,7 @@
       <c r="AE48" t="inlineStr"/>
       <c r="AF48" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6243,7 +6243,7 @@
       <c r="AE49" t="inlineStr"/>
       <c r="AF49" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6361,7 +6361,7 @@
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6479,7 +6479,7 @@
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
       <c r="AE52" t="inlineStr"/>
       <c r="AF52" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6715,7 +6715,7 @@
       <c r="AE53" t="inlineStr"/>
       <c r="AF53" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6833,7 +6833,7 @@
       <c r="AE54" t="inlineStr"/>
       <c r="AF54" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -6951,7 +6951,7 @@
       <c r="AE55" t="inlineStr"/>
       <c r="AF55" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7069,7 +7069,7 @@
       <c r="AE56" t="inlineStr"/>
       <c r="AF56" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7187,7 +7187,7 @@
       <c r="AE57" t="inlineStr"/>
       <c r="AF57" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7305,7 +7305,7 @@
       <c r="AE58" t="inlineStr"/>
       <c r="AF58" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7423,7 +7423,7 @@
       <c r="AE59" t="inlineStr"/>
       <c r="AF59" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7541,7 +7541,7 @@
       <c r="AE60" t="inlineStr"/>
       <c r="AF60" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7659,7 +7659,7 @@
       <c r="AE61" t="inlineStr"/>
       <c r="AF61" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7777,7 +7777,7 @@
       <c r="AE62" t="inlineStr"/>
       <c r="AF62" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -7895,7 +7895,7 @@
       <c r="AE63" t="inlineStr"/>
       <c r="AF63" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8013,7 +8013,7 @@
       <c r="AE64" t="inlineStr"/>
       <c r="AF64" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       <c r="AE65" t="inlineStr"/>
       <c r="AF65" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8249,7 +8249,7 @@
       <c r="AE66" t="inlineStr"/>
       <c r="AF66" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8367,7 +8367,7 @@
       <c r="AE67" t="inlineStr"/>
       <c r="AF67" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8485,7 +8485,7 @@
       <c r="AE68" t="inlineStr"/>
       <c r="AF68" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8603,7 +8603,7 @@
       <c r="AE69" t="inlineStr"/>
       <c r="AF69" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8721,7 +8721,7 @@
       <c r="AE70" t="inlineStr"/>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8839,7 +8839,7 @@
       <c r="AE71" t="inlineStr"/>
       <c r="AF71" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -8957,7 +8957,7 @@
       <c r="AE72" t="inlineStr"/>
       <c r="AF72" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9075,7 +9075,7 @@
       <c r="AE73" t="inlineStr"/>
       <c r="AF73" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9193,7 +9193,7 @@
       <c r="AE74" t="inlineStr"/>
       <c r="AF74" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9311,7 +9311,7 @@
       <c r="AE75" t="inlineStr"/>
       <c r="AF75" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9429,7 +9429,7 @@
       <c r="AE76" t="inlineStr"/>
       <c r="AF76" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9547,7 +9547,7 @@
       <c r="AE77" t="inlineStr"/>
       <c r="AF77" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9665,7 +9665,7 @@
       <c r="AE78" t="inlineStr"/>
       <c r="AF78" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9783,7 +9783,7 @@
       <c r="AE79" t="inlineStr"/>
       <c r="AF79" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -9901,7 +9901,7 @@
       <c r="AE80" t="inlineStr"/>
       <c r="AF80" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10019,7 +10019,7 @@
       <c r="AE81" t="inlineStr"/>
       <c r="AF81" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10137,7 +10137,7 @@
       <c r="AE82" t="inlineStr"/>
       <c r="AF82" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10255,7 +10255,7 @@
       <c r="AE83" t="inlineStr"/>
       <c r="AF83" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10373,7 +10373,7 @@
       <c r="AE84" t="inlineStr"/>
       <c r="AF84" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10491,7 +10491,7 @@
       <c r="AE85" t="inlineStr"/>
       <c r="AF85" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10609,7 +10609,7 @@
       <c r="AE86" t="inlineStr"/>
       <c r="AF86" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10727,7 +10727,7 @@
       <c r="AE87" t="inlineStr"/>
       <c r="AF87" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10845,7 +10845,7 @@
       <c r="AE88" t="inlineStr"/>
       <c r="AF88" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -10963,7 +10963,7 @@
       <c r="AE89" t="inlineStr"/>
       <c r="AF89" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11081,7 +11081,7 @@
       <c r="AE90" t="inlineStr"/>
       <c r="AF90" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11199,7 +11199,7 @@
       <c r="AE91" t="inlineStr"/>
       <c r="AF91" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11317,7 +11317,7 @@
       <c r="AE92" t="inlineStr"/>
       <c r="AF92" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11435,7 +11435,7 @@
       <c r="AE93" t="inlineStr"/>
       <c r="AF93" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11553,7 +11553,7 @@
       <c r="AE94" t="inlineStr"/>
       <c r="AF94" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11671,7 +11671,7 @@
       <c r="AE95" t="inlineStr"/>
       <c r="AF95" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11789,7 +11789,7 @@
       <c r="AE96" t="inlineStr"/>
       <c r="AF96" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -11907,7 +11907,7 @@
       <c r="AE97" t="inlineStr"/>
       <c r="AF97" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12025,7 +12025,7 @@
       <c r="AE98" t="inlineStr"/>
       <c r="AF98" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12143,7 +12143,7 @@
       <c r="AE99" t="inlineStr"/>
       <c r="AF99" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12261,7 +12261,7 @@
       <c r="AE100" t="inlineStr"/>
       <c r="AF100" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12379,7 +12379,7 @@
       <c r="AE101" t="inlineStr"/>
       <c r="AF101" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12497,7 +12497,7 @@
       <c r="AE102" t="inlineStr"/>
       <c r="AF102" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12615,7 +12615,7 @@
       <c r="AE103" t="inlineStr"/>
       <c r="AF103" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12733,7 +12733,7 @@
       <c r="AE104" t="inlineStr"/>
       <c r="AF104" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12851,7 +12851,7 @@
       <c r="AE105" t="inlineStr"/>
       <c r="AF105" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -12969,7 +12969,7 @@
       <c r="AE106" t="inlineStr"/>
       <c r="AF106" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13087,7 +13087,7 @@
       <c r="AE107" t="inlineStr"/>
       <c r="AF107" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13205,7 +13205,7 @@
       <c r="AE108" t="inlineStr"/>
       <c r="AF108" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13323,7 +13323,7 @@
       <c r="AE109" t="inlineStr"/>
       <c r="AF109" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13441,7 +13441,7 @@
       <c r="AE110" t="inlineStr"/>
       <c r="AF110" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13559,7 +13559,7 @@
       <c r="AE111" t="inlineStr"/>
       <c r="AF111" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13677,7 +13677,7 @@
       <c r="AE112" t="inlineStr"/>
       <c r="AF112" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13795,7 +13795,7 @@
       <c r="AE113" t="inlineStr"/>
       <c r="AF113" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -13913,7 +13913,7 @@
       <c r="AE114" t="inlineStr"/>
       <c r="AF114" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14031,7 +14031,7 @@
       <c r="AE115" t="inlineStr"/>
       <c r="AF115" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14149,7 +14149,7 @@
       <c r="AE116" t="inlineStr"/>
       <c r="AF116" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14267,7 +14267,7 @@
       <c r="AE117" t="inlineStr"/>
       <c r="AF117" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14385,7 +14385,7 @@
       <c r="AE118" t="inlineStr"/>
       <c r="AF118" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14503,7 +14503,7 @@
       <c r="AE119" t="inlineStr"/>
       <c r="AF119" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14621,7 +14621,7 @@
       <c r="AE120" t="inlineStr"/>
       <c r="AF120" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14739,7 +14739,7 @@
       <c r="AE121" t="inlineStr"/>
       <c r="AF121" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14857,7 +14857,7 @@
       <c r="AE122" t="inlineStr"/>
       <c r="AF122" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -14975,7 +14975,7 @@
       <c r="AE123" t="inlineStr"/>
       <c r="AF123" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15093,7 +15093,7 @@
       <c r="AE124" t="inlineStr"/>
       <c r="AF124" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15211,7 +15211,7 @@
       <c r="AE125" t="inlineStr"/>
       <c r="AF125" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15329,7 +15329,7 @@
       <c r="AE126" t="inlineStr"/>
       <c r="AF126" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15447,7 +15447,7 @@
       <c r="AE127" t="inlineStr"/>
       <c r="AF127" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15565,7 +15565,7 @@
       <c r="AE128" t="inlineStr"/>
       <c r="AF128" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15683,7 +15683,7 @@
       <c r="AE129" t="inlineStr"/>
       <c r="AF129" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15801,7 +15801,7 @@
       <c r="AE130" t="inlineStr"/>
       <c r="AF130" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -15919,7 +15919,7 @@
       <c r="AE131" t="inlineStr"/>
       <c r="AF131" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16037,7 +16037,7 @@
       <c r="AE132" t="inlineStr"/>
       <c r="AF132" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16155,7 +16155,7 @@
       <c r="AE133" t="inlineStr"/>
       <c r="AF133" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16273,7 +16273,7 @@
       <c r="AE134" t="inlineStr"/>
       <c r="AF134" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16391,7 +16391,7 @@
       <c r="AE135" t="inlineStr"/>
       <c r="AF135" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16509,7 +16509,7 @@
       <c r="AE136" t="inlineStr"/>
       <c r="AF136" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16627,7 +16627,7 @@
       <c r="AE137" t="inlineStr"/>
       <c r="AF137" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16745,7 +16745,7 @@
       <c r="AE138" t="inlineStr"/>
       <c r="AF138" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16863,7 +16863,7 @@
       <c r="AE139" t="inlineStr"/>
       <c r="AF139" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -16981,7 +16981,7 @@
       <c r="AE140" t="inlineStr"/>
       <c r="AF140" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -17099,7 +17099,7 @@
       <c r="AE141" t="inlineStr"/>
       <c r="AF141" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -17217,7 +17217,7 @@
       <c r="AE142" t="inlineStr"/>
       <c r="AF142" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -17335,7 +17335,7 @@
       <c r="AE143" t="inlineStr"/>
       <c r="AF143" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -17453,7 +17453,7 @@
       <c r="AE144" t="inlineStr"/>
       <c r="AF144" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>
@@ -17571,7 +17571,7 @@
       <c r="AE145" t="inlineStr"/>
       <c r="AF145" t="inlineStr">
         <is>
-          <t>28/01/2026 16:16:21</t>
+          <t>28/01/2026 21:50:58</t>
         </is>
       </c>
     </row>

</xml_diff>